<commit_message>
updated forms for pilot
</commit_message>
<xml_diff>
--- a/labstatus.xlsx
+++ b/labstatus.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="63">
   <si>
     <t>type</t>
   </si>
@@ -78,28 +78,40 @@
     <t>quick search('facilities', 'matches', 'region', ${region})</t>
   </si>
   <si>
+    <t>barcode</t>
+  </si>
+  <si>
+    <t>stid</t>
+  </si>
+  <si>
+    <t>Sample Tracking ID</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>labid</t>
+  </si>
+  <si>
+    <t>Lab ID</t>
+  </si>
+  <si>
+    <t>dateTime</t>
+  </si>
+  <si>
+    <t>labtime</t>
+  </si>
+  <si>
+    <t>Status Timestamp</t>
+  </si>
+  <si>
     <t>begin repeat</t>
   </si>
   <si>
     <t>srepeat</t>
   </si>
   <si>
-    <t>New Sample</t>
-  </si>
-  <si>
-    <t>barcode</t>
-  </si>
-  <si>
-    <t>stid</t>
-  </si>
-  <si>
-    <t>ST Barcode</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>labid</t>
+    <t>New Sample Test</t>
   </si>
   <si>
     <t>select_one labstatus</t>
@@ -278,10 +290,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/worksheetdrawing.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
-</file>
-
 <file path=xl/drawings/worksheetdrawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
@@ -290,7 +298,11 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
-<file path=xl/worksheets/sheet.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/worksheetdrawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
+<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -349,7 +361,6 @@
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
@@ -361,7 +372,6 @@
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
@@ -415,58 +425,56 @@
       <c r="B9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="5"/>
+      <c r="D9" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="E9" s="6"/>
     </row>
     <row r="10">
       <c r="A10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="4" t="s">
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="7" t="s">
         <v>27</v>
-      </c>
-      <c r="E10" s="6"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="4" t="s">
-        <v>24</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>27</v>
+      <c r="C11" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="E11" s="4"/>
     </row>
     <row r="12">
-      <c r="A12" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" s="7" t="s">
+      <c r="A12" s="4" t="s">
         <v>30</v>
       </c>
+      <c r="B12" s="4" t="s">
+        <v>31</v>
+      </c>
       <c r="C12" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E12" s="7" t="s">
         <v>32</v>
       </c>
+      <c r="D12" s="5"/>
+      <c r="E12" s="6"/>
     </row>
     <row r="13">
       <c r="A13" s="7" t="s">
@@ -479,7 +487,7 @@
         <v>35</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>36</v>
@@ -489,46 +497,61 @@
       <c r="A14" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="7" t="s">
         <v>38</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="8" t="s">
+      <c r="D14" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="7" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
+      <c r="B15" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>43</v>
+      </c>
       <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
+      <c r="E15" s="8" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>27</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="4"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -537,7 +560,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -551,7 +574,7 @@
         <v>14</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>14</v>
@@ -562,7 +585,7 @@
         <v>18</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>18</v>
@@ -570,46 +593,46 @@
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="7" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="7" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="7" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -617,7 +640,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -626,18 +649,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="9" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="10" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
better lab status form
</commit_message>
<xml_diff>
--- a/labstatus.xlsx
+++ b/labstatus.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="66">
   <si>
     <t>type</t>
   </si>
@@ -160,6 +160,15 @@
   </si>
   <si>
     <t>GPS Coordinates</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>raw_xml</t>
+  </si>
+  <si>
+    <t>Original Disa Labs XML submission</t>
   </si>
   <si>
     <t>list name</t>
@@ -208,7 +217,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -226,6 +235,7 @@
     <font>
       <name val="Arial"/>
     </font>
+    <font/>
     <font>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -250,7 +260,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -276,10 +286,13 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
   </cellXfs>
@@ -546,6 +559,17 @@
       </c>
       <c r="D17" s="4"/>
     </row>
+    <row r="18">
+      <c r="A18" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>51</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -560,7 +584,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -574,7 +598,7 @@
         <v>14</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>14</v>
@@ -585,7 +609,7 @@
         <v>18</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>18</v>
@@ -593,13 +617,13 @@
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5">
@@ -607,10 +631,10 @@
         <v>34</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6">
@@ -618,10 +642,10 @@
         <v>38</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7">
@@ -629,10 +653,10 @@
         <v>42</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -648,18 +672,18 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>61</v>
+      <c r="A1" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="B2" s="10" t="s">
+      <c r="A2" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>

<commit_message>
re-included rawxml field with extended string length
</commit_message>
<xml_diff>
--- a/labstatus.xlsx
+++ b/labstatus.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="67">
   <si>
     <t>type</t>
   </si>
@@ -30,6 +30,9 @@
     <t>appearance</t>
   </si>
   <si>
+    <t>bind::odk-length</t>
+  </si>
+  <si>
     <t>start</t>
   </si>
   <si>
@@ -160,6 +163,15 @@
   </si>
   <si>
     <t>GPS Coordinates</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>rawxml</t>
+  </si>
+  <si>
+    <t>Disa Labs Raw XML submission</t>
   </si>
   <si>
     <t>list name</t>
@@ -208,7 +220,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -224,19 +236,30 @@
       <name val="Arial"/>
     </font>
     <font>
+      <b/>
+      <color rgb="FF000000"/>
+    </font>
+    <font>
       <name val="Arial"/>
     </font>
+    <font/>
     <font>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -250,7 +273,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -263,23 +286,29 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
   </cellXfs>
@@ -328,223 +357,240 @@
       <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
+      <c r="A2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
     </row>
     <row r="3">
-      <c r="A3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
+      <c r="A3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
+      <c r="A4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
     </row>
     <row r="5">
-      <c r="A5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
+      <c r="A5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
     </row>
     <row r="6">
-      <c r="A6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="4" t="s">
+      <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="B6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="4" t="s">
+      <c r="C6" s="5" t="s">
         <v>12</v>
       </c>
+      <c r="D6" s="7"/>
+      <c r="E6" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="4" t="s">
+      <c r="A7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="B7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4" t="s">
+      <c r="C7" s="5" t="s">
         <v>16</v>
       </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="4" t="s">
+      <c r="A8" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="B8" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4" t="s">
+      <c r="C8" s="5" t="s">
         <v>20</v>
       </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="4" t="s">
+      <c r="A9" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="B9" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="C9" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="6"/>
+      <c r="D9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="7"/>
     </row>
     <row r="10">
-      <c r="A10" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="7" t="s">
+      <c r="A10" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" s="4"/>
+      <c r="E10" s="5"/>
     </row>
     <row r="11">
-      <c r="A11" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="7" t="s">
+      <c r="A11" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="B11" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E11" s="4"/>
+      <c r="C11" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="5"/>
     </row>
     <row r="12">
-      <c r="A12" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="4" t="s">
+      <c r="A12" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="B12" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="6"/>
+      <c r="C12" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="6"/>
+      <c r="E12" s="7"/>
     </row>
     <row r="13">
-      <c r="A13" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" s="7" t="s">
+      <c r="A13" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="B13" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D13" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E13" s="7" t="s">
+      <c r="C13" s="8" t="s">
         <v>36</v>
       </c>
+      <c r="D13" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="14">
-      <c r="A14" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="B14" s="7" t="s">
+      <c r="A14" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="B14" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E14" s="7" t="s">
+      <c r="C14" s="8" t="s">
         <v>40</v>
       </c>
+      <c r="D14" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="15">
-      <c r="A15" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B15" s="8" t="s">
+      <c r="A15" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="B15" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="8" t="s">
+      <c r="C15" s="8" t="s">
         <v>44</v>
       </c>
+      <c r="D15" s="6"/>
+      <c r="E15" s="9" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="16">
-      <c r="A16" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
+      <c r="A16" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
     </row>
     <row r="17">
-      <c r="A17" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B17" s="4" t="s">
+      <c r="A17" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="B17" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D17" s="4"/>
+      <c r="C17" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="5"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="F18" s="10">
+        <v>16000.0</v>
+      </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -560,7 +606,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -570,69 +616,69 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>14</v>
+      <c r="A2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>18</v>
+      <c r="A3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>52</v>
+      <c r="A4" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>55</v>
+      <c r="A5" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>57</v>
+      <c r="A6" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>59</v>
+      <c r="A7" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -648,19 +694,19 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>61</v>
+      <c r="A1" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>34</v>
+      <c r="A2" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated forms with labs
</commit_message>
<xml_diff>
--- a/labstatus.xlsx
+++ b/labstatus.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="63">
   <si>
     <t>type</t>
   </si>
@@ -45,28 +45,16 @@
     <t>simserial</t>
   </si>
   <si>
-    <t>select_one rider</t>
-  </si>
-  <si>
-    <t>person</t>
-  </si>
-  <si>
-    <t>Lab Person</t>
-  </si>
-  <si>
-    <t>quick search('riders')</t>
-  </si>
-  <si>
     <t>select_one region</t>
   </si>
   <si>
     <t>region</t>
   </si>
   <si>
-    <t>Region</t>
-  </si>
-  <si>
-    <t>quick search('regions')</t>
+    <t>Facility Lab</t>
+  </si>
+  <si>
+    <t>quick search('labs')</t>
   </si>
   <si>
     <t>select_one facility</t>
@@ -177,18 +165,15 @@
     <t>list name</t>
   </si>
   <si>
-    <t>region_key</t>
+    <t>lab_key</t>
+  </si>
+  <si>
+    <t>lab</t>
   </si>
   <si>
     <t>facility_key</t>
   </si>
   <si>
-    <t>rider</t>
-  </si>
-  <si>
-    <t>rider_key</t>
-  </si>
-  <si>
     <t>status_key</t>
   </si>
   <si>
@@ -211,6 +196,9 @@
   </si>
   <si>
     <t>form_id</t>
+  </si>
+  <si>
+    <t>version</t>
   </si>
   <si>
     <t>Lab Status</t>
@@ -273,7 +261,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -308,8 +296,14 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -409,14 +403,14 @@
       <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="5" t="s">
+      <c r="D6" s="5"/>
+      <c r="E6" s="8" t="s">
         <v>13</v>
       </c>
     </row>
@@ -442,71 +436,73 @@
       <c r="B8" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5" t="s">
+      <c r="D8" s="5" t="s">
         <v>21</v>
       </c>
+      <c r="E8" s="7"/>
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="C9" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="D9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="B10" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="7"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="8" t="s">
+      <c r="C10" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="D10" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="5"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="5"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="8" t="s">
+      <c r="B11" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="C11" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="D11" s="6"/>
+      <c r="E11" s="7"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E11" s="5"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="5" t="s">
+      <c r="B12" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="C12" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="D12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="7"/>
     </row>
     <row r="13">
       <c r="A13" s="8" t="s">
@@ -519,7 +515,7 @@
         <v>36</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E13" s="8" t="s">
         <v>37</v>
@@ -529,66 +525,49 @@
       <c r="A14" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="9" t="s">
         <v>39</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D14" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E14" s="8" t="s">
+      <c r="D14" s="6"/>
+      <c r="E14" s="9" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>44</v>
-      </c>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
       <c r="D15" s="6"/>
-      <c r="E15" s="9" t="s">
-        <v>45</v>
-      </c>
+      <c r="E15" s="6"/>
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="5"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="5" t="s">
+      <c r="B17" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="C17" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D17" s="5"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="F18" s="10">
+      <c r="F17" s="10">
         <v>16000.0</v>
       </c>
     </row>
@@ -606,7 +585,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -616,36 +595,36 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>15</v>
+      <c r="A2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>56</v>
+      <c r="A4" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="5">
@@ -653,10 +632,10 @@
         <v>35</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6">
@@ -664,21 +643,10 @@
         <v>39</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -695,18 +663,24 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="11" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>65</v>
+        <v>60</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>35</v>
+      <c r="A2" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="14">
+        <v>2.016041301E9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>